<commit_message>
Added more robust input validation to dates
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/CashCreditDepositReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/CashCreditDepositReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAB6CC3D-6873-42B1-A85C-1B945BD594D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF923541-568C-40D5-8ABC-84A374F2F054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{B91A9AAF-25B5-4F7D-95ED-5B93A3AD9522}"/>
+    <workbookView xWindow="31050" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{7C892564-4C89-4D4D-BEC2-0A81D07E9D06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Cash Deposit for 2021-7-2021</t>
+    <t>Cash Deposit for 2001-12-12</t>
   </si>
   <si>
-    <t>Credit Deposit for 2021-7-2021</t>
+    <t>Credit Deposit for 2001-12-12</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0282000-3C3F-4006-87D0-A8788C59E5C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2F647B-0C63-4BAF-AB30-B275251FF15C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
fixed deposit report. Now only accounts for transactions that are purchases.
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/CashCreditDepositReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/CashCreditDepositReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016be9303c01b4f8/Documents/SCHOOL STUFF/05 Summer 2021/Capstone/malloyethan11/report_creation_program/report_creation_program/report_creation_program/bin/Debug/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF923541-568C-40D5-8ABC-84A374F2F054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EAD0ADB-1E51-4EA4-AB21-EC924843E4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{7C892564-4C89-4D4D-BEC2-0A81D07E9D06}"/>
+    <workbookView xWindow="-26490" yWindow="1005" windowWidth="22980" windowHeight="13770" xr2:uid="{68EFFBB0-3B8B-4B1D-8CE9-5EA8587A025A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Cash Deposit for 2001-12-12</t>
+    <t>Cash Deposit for 2021-07-16</t>
   </si>
   <si>
-    <t>Credit Deposit for 2001-12-12</t>
+    <t>Credit Deposit for 2021-07-16</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2F647B-0C63-4BAF-AB30-B275251FF15C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7252B6-6C69-4698-AE62-42ADFD606C0D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -407,10 +407,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>520.52</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>437.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>